<commit_message>
Modify hlm dataloader to load erosion data and soil data in same excel file
</commit_message>
<xml_diff>
--- a/data/hlm/predict_erosion_data.xlsx
+++ b/data/hlm/predict_erosion_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\PyProjects\simpleLearning\data\hlm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131C6D9C-9F75-494D-964E-EEE35ADEBBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861DB68-0A04-4205-A6B2-E25F530C6290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="528" windowWidth="13068" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9276" yWindow="912" windowWidth="13068" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="erosion" sheetId="1" r:id="rId1"/>
+    <sheet name="soil" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>站点</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +37,38 @@
   </si>
   <si>
     <t>埋存时间(年)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PH值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全氮含量(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>碳酸根离子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>硫酸根离子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镁离子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钾离子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钠离子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土壤电阻(Ω)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -363,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -429,4 +462,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFB7311-409E-485C-AA04-CFD7F4120BDF}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>6.75</v>
+      </c>
+      <c r="C2">
+        <v>0.109</v>
+      </c>
+      <c r="D2">
+        <v>1.26E-2</v>
+      </c>
+      <c r="E2">
+        <v>1.18E-2</v>
+      </c>
+      <c r="F2">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="G2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="I2">
+        <v>32.9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>